<commit_message>
Fixed errors at level A and B
Inconsistent indexing/ naming of Level A and B tasks lead to numerous errors that needed to be fixed.  Most inconsistencies related to whether task numbers should be unique across all tasks or only w/n each level.  New policy is that all task numbers are unique. This change affects how a given task is indexed within the list of tasks for each level.
</commit_message>
<xml_diff>
--- a/levelAGenerator.xlsx
+++ b/levelAGenerator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10980" windowHeight="7590"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -221,31 +221,31 @@
     <t>TaskID</t>
   </si>
   <si>
-    <t>0-A-2</t>
-  </si>
-  <si>
-    <t>0-A-1</t>
-  </si>
-  <si>
-    <t>0-A-0</t>
-  </si>
-  <si>
-    <t>0-B-2</t>
-  </si>
-  <si>
-    <t>0-B-1</t>
-  </si>
-  <si>
-    <t>0-B-0</t>
-  </si>
-  <si>
-    <t>0-C-2</t>
-  </si>
-  <si>
-    <t>0-C-1</t>
-  </si>
-  <si>
-    <t>0-C-0</t>
+    <t>8-A-2</t>
+  </si>
+  <si>
+    <t>8-A-1</t>
+  </si>
+  <si>
+    <t>8-A-0</t>
+  </si>
+  <si>
+    <t>8-B-2</t>
+  </si>
+  <si>
+    <t>8-B-1</t>
+  </si>
+  <si>
+    <t>8-B-0</t>
+  </si>
+  <si>
+    <t>8-C-2</t>
+  </si>
+  <si>
+    <t>8-C-1</t>
+  </si>
+  <si>
+    <t>8-C-0</t>
   </si>
 </sst>
 </file>
@@ -584,7 +584,7 @@
   <dimension ref="A1:BV9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,220 +600,220 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
       <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" t="s">
         <v>66</v>
       </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>14</v>
-      </c>
       <c r="S1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" t="s">
         <v>67</v>
       </c>
-      <c r="T1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" t="s">
-        <v>15</v>
-      </c>
-      <c r="V1" t="s">
-        <v>16</v>
-      </c>
-      <c r="W1" t="s">
-        <v>17</v>
-      </c>
-      <c r="X1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>20</v>
-      </c>
       <c r="AA1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH1" t="s">
         <v>68</v>
       </c>
-      <c r="AB1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>28</v>
-      </c>
       <c r="AI1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP1" t="s">
         <v>69</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>35</v>
-      </c>
       <c r="AQ1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AX1" t="s">
         <v>70</v>
       </c>
-      <c r="AR1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>42</v>
-      </c>
       <c r="AY1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>44</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BF1" t="s">
         <v>71</v>
       </c>
-      <c r="AZ1" t="s">
-        <v>43</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>44</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>45</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>46</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>47</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>48</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>49</v>
-      </c>
       <c r="BG1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN1" t="s">
         <v>72</v>
       </c>
-      <c r="BH1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>56</v>
-      </c>
       <c r="BO1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BV1" t="s">
         <v>73</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:74" x14ac:dyDescent="0.25">
@@ -828,31 +828,31 @@
       </c>
       <c r="D2" s="1">
         <f ca="1">RANDBETWEEN(MIN($C2, D3)*100, ($C2+D3)*100)/100</f>
-        <v>0.23</v>
+        <v>0.16</v>
       </c>
       <c r="E2" s="1">
         <f ca="1">RANDBETWEEN(MIN($C2, E$4)*100, ($C2+E$4)*100)/100</f>
-        <v>0.27</v>
+        <v>0.24</v>
       </c>
       <c r="F2" s="1">
         <f ca="1">RANDBETWEEN(MIN($C2, F$5)*100, ($C2+F$5)*100)/100</f>
-        <v>0.42</v>
+        <v>0.1</v>
       </c>
       <c r="G2" s="1">
         <f ca="1">RANDBETWEEN(MIN($C2, G$6)*100, ($C2+G$6)*100)/100</f>
-        <v>0.16</v>
+        <v>0.59</v>
       </c>
       <c r="H2" s="1">
         <f ca="1">RANDBETWEEN(MIN($C2, H$7)*100, ($C2+H$7)*100)/100</f>
-        <v>0.28999999999999998</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I2" s="1">
         <f ca="1">RANDBETWEEN(MIN($C2, I$8)*100, ($C2+I$8)*100)/100</f>
-        <v>0.67</v>
+        <v>0.25</v>
       </c>
       <c r="J2" s="1">
         <f ca="1">RANDBETWEEN(MIN($C2, J$9)*100, ($C2+J9)*100)/100</f>
-        <v>0.17</v>
+        <v>0.61</v>
       </c>
       <c r="K2" s="3">
         <f>C2*1.25</f>
@@ -860,31 +860,31 @@
       </c>
       <c r="L2" s="1">
         <f t="shared" ref="L2:R2" ca="1" si="0">D2*1.25</f>
-        <v>0.28750000000000003</v>
+        <v>0.2</v>
       </c>
       <c r="M2" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33750000000000002</v>
+        <v>0.3</v>
       </c>
       <c r="N2" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52500000000000002</v>
+        <v>0.125</v>
       </c>
       <c r="O2" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>0.73749999999999993</v>
       </c>
       <c r="P2" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.36249999999999999</v>
+        <v>0.6875</v>
       </c>
       <c r="Q2" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83750000000000002</v>
+        <v>0.3125</v>
       </c>
       <c r="R2" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21250000000000002</v>
+        <v>0.76249999999999996</v>
       </c>
       <c r="S2" s="1">
         <f>C2*1.5</f>
@@ -892,31 +892,31 @@
       </c>
       <c r="T2" s="1">
         <f t="shared" ref="T2:Z9" ca="1" si="1">D2*1.5</f>
-        <v>0.34500000000000003</v>
+        <v>0.24</v>
       </c>
       <c r="U2" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.40500000000000003</v>
+        <v>0.36</v>
       </c>
       <c r="V2" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="W2" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="X2" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43499999999999994</v>
+        <v>0.82500000000000007</v>
       </c>
       <c r="Y2" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0050000000000001</v>
+        <v>0.375</v>
       </c>
       <c r="Z2" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.255</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="AA2" s="1">
         <f>C2/2</f>
@@ -924,31 +924,31 @@
       </c>
       <c r="AB2" s="1">
         <f t="shared" ref="AB2:AX9" ca="1" si="2">D2/2</f>
-        <v>0.115</v>
+        <v>0.08</v>
       </c>
       <c r="AC2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.13500000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="AD2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.21</v>
+        <v>0.05</v>
       </c>
       <c r="AE2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.08</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="AF2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.14499999999999999</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="AG2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.33500000000000002</v>
+        <v>0.125</v>
       </c>
       <c r="AH2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8.5000000000000006E-2</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="AI2" s="1">
         <f t="shared" si="2"/>
@@ -956,31 +956,31 @@
       </c>
       <c r="AJ2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.14375000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="AK2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.16875000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="AL2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.26250000000000001</v>
+        <v>6.25E-2</v>
       </c>
       <c r="AM2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.1</v>
+        <v>0.36874999999999997</v>
       </c>
       <c r="AN2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.18124999999999999</v>
+        <v>0.34375</v>
       </c>
       <c r="AO2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.41875000000000001</v>
+        <v>0.15625</v>
       </c>
       <c r="AP2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.10625000000000001</v>
+        <v>0.38124999999999998</v>
       </c>
       <c r="AQ2" s="1">
         <f t="shared" si="2"/>
@@ -988,31 +988,31 @@
       </c>
       <c r="AR2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.17250000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="AS2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.20250000000000001</v>
+        <v>0.18</v>
       </c>
       <c r="AT2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.315</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="AU2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.12</v>
+        <v>0.4425</v>
       </c>
       <c r="AV2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.21749999999999997</v>
+        <v>0.41250000000000003</v>
       </c>
       <c r="AW2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.50250000000000006</v>
+        <v>0.1875</v>
       </c>
       <c r="AX2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.1275</v>
+        <v>0.45750000000000002</v>
       </c>
       <c r="AY2" s="1">
         <f>C2/4</f>
@@ -1020,31 +1020,31 @@
       </c>
       <c r="AZ2" s="1">
         <f t="shared" ref="AZ2:BV9" ca="1" si="3">D2/4</f>
-        <v>5.7500000000000002E-2</v>
+        <v>0.04</v>
       </c>
       <c r="BA2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>6.7500000000000004E-2</v>
+        <v>0.06</v>
       </c>
       <c r="BB2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.105</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="BC2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.04</v>
+        <v>0.14749999999999999</v>
       </c>
       <c r="BD2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>7.2499999999999995E-2</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="BE2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.16750000000000001</v>
+        <v>6.25E-2</v>
       </c>
       <c r="BF2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4.2500000000000003E-2</v>
+        <v>0.1525</v>
       </c>
       <c r="BG2" s="1">
         <f t="shared" si="3"/>
@@ -1052,31 +1052,31 @@
       </c>
       <c r="BH2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>7.1875000000000008E-2</v>
+        <v>0.05</v>
       </c>
       <c r="BI2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>8.4375000000000006E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="BJ2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.13125000000000001</v>
+        <v>3.125E-2</v>
       </c>
       <c r="BK2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.05</v>
+        <v>0.18437499999999998</v>
       </c>
       <c r="BL2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>9.0624999999999997E-2</v>
+        <v>0.171875</v>
       </c>
       <c r="BM2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.20937500000000001</v>
+        <v>7.8125E-2</v>
       </c>
       <c r="BN2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>5.3125000000000006E-2</v>
+        <v>0.19062499999999999</v>
       </c>
       <c r="BO2" s="1">
         <f t="shared" si="3"/>
@@ -1084,31 +1084,31 @@
       </c>
       <c r="BP2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>8.6250000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="BQ2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.10125000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="BR2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1575</v>
+        <v>3.7500000000000006E-2</v>
       </c>
       <c r="BS2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.06</v>
+        <v>0.22125</v>
       </c>
       <c r="BT2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.10874999999999999</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="BU2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.25125000000000003</v>
+        <v>9.375E-2</v>
       </c>
       <c r="BV2" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>6.3750000000000001E-2</v>
+        <v>0.22875000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:74" x14ac:dyDescent="0.25">
@@ -1120,38 +1120,38 @@
       </c>
       <c r="C3" s="1">
         <f ca="1">D2</f>
-        <v>0.23</v>
+        <v>0.16</v>
       </c>
       <c r="D3" s="2">
         <v>0.2</v>
       </c>
       <c r="E3" s="1">
         <f ca="1">RANDBETWEEN(MIN($D3, E$4)*100, ($D3+E$4)*100)/100</f>
-        <v>0.49</v>
+        <v>0.24</v>
       </c>
       <c r="F3" s="1">
         <f ca="1">RANDBETWEEN(MIN($D3, F$5)*100, ($D3+F$5)*100)/100</f>
-        <v>0.46</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="G3" s="1">
         <f ca="1">RANDBETWEEN(MIN(D3, G6)*100, ($D3+G6)*100)/100</f>
-        <v>0.56000000000000005</v>
+        <v>0.51</v>
       </c>
       <c r="H3" s="1">
         <f ca="1">RANDBETWEEN(MIN($D3, H7)*100, ($D3+H7)*100)/100</f>
-        <v>0.41</v>
+        <v>0.78</v>
       </c>
       <c r="I3" s="1">
         <f ca="1">RANDBETWEEN(MIN($D3, I8)*100, ($D3+I8)*100)/100</f>
-        <v>0.63</v>
+        <v>0.59</v>
       </c>
       <c r="J3" s="1">
         <f ca="1">RANDBETWEEN(MIN($D3, J9)*100, ($D3+J9)*100)/100</f>
-        <v>0.47</v>
+        <v>0.37</v>
       </c>
       <c r="K3" s="3">
         <f t="shared" ref="K3:K9" ca="1" si="4">C3*1.25</f>
-        <v>0.28750000000000003</v>
+        <v>0.2</v>
       </c>
       <c r="L3" s="1">
         <f t="shared" ref="L3:L9" si="5">D3*1.25</f>
@@ -1159,31 +1159,31 @@
       </c>
       <c r="M3" s="1">
         <f t="shared" ref="M3:M9" ca="1" si="6">E3*1.25</f>
-        <v>0.61250000000000004</v>
+        <v>0.3</v>
       </c>
       <c r="N3" s="1">
         <f t="shared" ref="N3:N9" ca="1" si="7">F3*1.25</f>
-        <v>0.57500000000000007</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="O3" s="1">
         <f t="shared" ref="O3:O9" ca="1" si="8">G3*1.25</f>
-        <v>0.70000000000000007</v>
+        <v>0.63749999999999996</v>
       </c>
       <c r="P3" s="1">
         <f t="shared" ref="P3:P9" ca="1" si="9">H3*1.25</f>
-        <v>0.51249999999999996</v>
+        <v>0.97500000000000009</v>
       </c>
       <c r="Q3" s="1">
         <f t="shared" ref="Q3:Q9" ca="1" si="10">I3*1.25</f>
-        <v>0.78749999999999998</v>
+        <v>0.73749999999999993</v>
       </c>
       <c r="R3" s="1">
         <f t="shared" ref="R3:R9" ca="1" si="11">J3*1.25</f>
-        <v>0.58749999999999991</v>
+        <v>0.46250000000000002</v>
       </c>
       <c r="S3" s="1">
         <f t="shared" ref="S3:S9" ca="1" si="12">C3*1.5</f>
-        <v>0.34500000000000003</v>
+        <v>0.24</v>
       </c>
       <c r="T3" s="1">
         <f t="shared" si="1"/>
@@ -1191,31 +1191,31 @@
       </c>
       <c r="U3" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.73499999999999999</v>
+        <v>0.36</v>
       </c>
       <c r="V3" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69000000000000006</v>
+        <v>0.84000000000000008</v>
       </c>
       <c r="W3" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.84000000000000008</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="X3" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61499999999999999</v>
+        <v>1.17</v>
       </c>
       <c r="Y3" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94500000000000006</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="Z3" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70499999999999996</v>
+        <v>0.55499999999999994</v>
       </c>
       <c r="AA3" s="1">
         <f t="shared" ref="AA3:AA9" ca="1" si="13">C3/2</f>
-        <v>0.115</v>
+        <v>0.08</v>
       </c>
       <c r="AB3" s="1">
         <f t="shared" si="2"/>
@@ -1223,31 +1223,31 @@
       </c>
       <c r="AC3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.245</v>
+        <v>0.12</v>
       </c>
       <c r="AD3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.23</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AE3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.28000000000000003</v>
+        <v>0.255</v>
       </c>
       <c r="AF3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.20499999999999999</v>
+        <v>0.39</v>
       </c>
       <c r="AG3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.315</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="AH3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.23499999999999999</v>
+        <v>0.185</v>
       </c>
       <c r="AI3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.14375000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" si="2"/>
@@ -1255,31 +1255,31 @@
       </c>
       <c r="AK3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.30625000000000002</v>
+        <v>0.15</v>
       </c>
       <c r="AL3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.28750000000000003</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="AM3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.35000000000000003</v>
+        <v>0.31874999999999998</v>
       </c>
       <c r="AN3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.25624999999999998</v>
+        <v>0.48750000000000004</v>
       </c>
       <c r="AO3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.39374999999999999</v>
+        <v>0.36874999999999997</v>
       </c>
       <c r="AP3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.29374999999999996</v>
+        <v>0.23125000000000001</v>
       </c>
       <c r="AQ3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.17250000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="AR3" s="1">
         <f t="shared" si="2"/>
@@ -1287,31 +1287,31 @@
       </c>
       <c r="AS3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.36749999999999999</v>
+        <v>0.18</v>
       </c>
       <c r="AT3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.34500000000000003</v>
+        <v>0.42000000000000004</v>
       </c>
       <c r="AU3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.42000000000000004</v>
+        <v>0.38250000000000001</v>
       </c>
       <c r="AV3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.3075</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="AW3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.47250000000000003</v>
+        <v>0.4425</v>
       </c>
       <c r="AX3" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.35249999999999998</v>
+        <v>0.27749999999999997</v>
       </c>
       <c r="AY3" s="1">
         <f t="shared" ref="AY3:AY9" ca="1" si="14">C3/4</f>
-        <v>5.7500000000000002E-2</v>
+        <v>0.04</v>
       </c>
       <c r="AZ3" s="1">
         <f t="shared" si="3"/>
@@ -1319,31 +1319,31 @@
       </c>
       <c r="BA3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1225</v>
+        <v>0.06</v>
       </c>
       <c r="BB3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.115</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="BC3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14000000000000001</v>
+        <v>0.1275</v>
       </c>
       <c r="BD3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.10249999999999999</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="BE3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1575</v>
+        <v>0.14749999999999999</v>
       </c>
       <c r="BF3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.11749999999999999</v>
+        <v>9.2499999999999999E-2</v>
       </c>
       <c r="BG3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>7.1875000000000008E-2</v>
+        <v>0.05</v>
       </c>
       <c r="BH3" s="1">
         <f t="shared" si="3"/>
@@ -1351,31 +1351,31 @@
       </c>
       <c r="BI3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.15312500000000001</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="BJ3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14375000000000002</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="BK3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.17500000000000002</v>
+        <v>0.15937499999999999</v>
       </c>
       <c r="BL3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.12812499999999999</v>
+        <v>0.24375000000000002</v>
       </c>
       <c r="BM3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.19687499999999999</v>
+        <v>0.18437499999999998</v>
       </c>
       <c r="BN3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14687499999999998</v>
+        <v>0.11562500000000001</v>
       </c>
       <c r="BO3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>8.6250000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="BP3" s="1">
         <f t="shared" si="3"/>
@@ -1383,27 +1383,27 @@
       </c>
       <c r="BQ3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.18375</v>
+        <v>0.09</v>
       </c>
       <c r="BR3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.17250000000000001</v>
+        <v>0.21000000000000002</v>
       </c>
       <c r="BS3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.21000000000000002</v>
+        <v>0.19125</v>
       </c>
       <c r="BT3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.15375</v>
+        <v>0.29249999999999998</v>
       </c>
       <c r="BU3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.23625000000000002</v>
+        <v>0.22125</v>
       </c>
       <c r="BV3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.17624999999999999</v>
+        <v>0.13874999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:74" x14ac:dyDescent="0.25">
@@ -1415,42 +1415,42 @@
       </c>
       <c r="C4" s="1">
         <f ca="1">E2</f>
-        <v>0.27</v>
+        <v>0.24</v>
       </c>
       <c r="D4" s="1">
         <f ca="1">E3</f>
-        <v>0.49</v>
+        <v>0.24</v>
       </c>
       <c r="E4" s="2">
         <v>0.3</v>
       </c>
       <c r="F4" s="1">
         <f ca="1">RANDBETWEEN(MIN($E4, F$5)*100, ($E4+F$5)*100)/100</f>
-        <v>0.35</v>
+        <v>0.43</v>
       </c>
       <c r="G4" s="1">
         <f ca="1">RANDBETWEEN(MIN($E4, G6)*100, ($E4+G6)*100)/100</f>
-        <v>0.45</v>
+        <v>0.64</v>
       </c>
       <c r="H4" s="1">
         <f ca="1">RANDBETWEEN(MIN($E4, H7)*100, ($E4+H7)*100)/100</f>
-        <v>0.73</v>
+        <v>0.54</v>
       </c>
       <c r="I4" s="1">
         <f ca="1">RANDBETWEEN(MIN($E4, I8)*100, ($E4+I8)*100)/100</f>
-        <v>0.44</v>
+        <v>0.63</v>
       </c>
       <c r="J4" s="1">
         <f ca="1">RANDBETWEEN(MIN($E4, J9)*100, ($E4+J9)*100)/100</f>
-        <v>0.57999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="K4" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.33750000000000002</v>
+        <v>0.3</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0.61250000000000004</v>
+        <v>0.3</v>
       </c>
       <c r="M4" s="1">
         <f t="shared" si="6"/>
@@ -1458,31 +1458,31 @@
       </c>
       <c r="N4" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>0.4375</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="O4" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>0.5625</v>
+        <v>0.8</v>
       </c>
       <c r="P4" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.91249999999999998</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="Q4" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>0.55000000000000004</v>
+        <v>0.78749999999999998</v>
       </c>
       <c r="R4" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0.72499999999999998</v>
+        <v>0.625</v>
       </c>
       <c r="S4" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>0.40500000000000003</v>
+        <v>0.36</v>
       </c>
       <c r="T4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.73499999999999999</v>
+        <v>0.36</v>
       </c>
       <c r="U4" s="1">
         <f t="shared" si="1"/>
@@ -1490,31 +1490,31 @@
       </c>
       <c r="V4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52499999999999991</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="W4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67500000000000004</v>
+        <v>0.96</v>
       </c>
       <c r="X4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.095</v>
+        <v>0.81</v>
       </c>
       <c r="Y4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.66</v>
+        <v>0.94500000000000006</v>
       </c>
       <c r="Z4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86999999999999988</v>
+        <v>0.75</v>
       </c>
       <c r="AA4" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>0.13500000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="AB4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.245</v>
+        <v>0.12</v>
       </c>
       <c r="AC4" s="1">
         <f t="shared" si="2"/>
@@ -1522,31 +1522,31 @@
       </c>
       <c r="AD4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.17499999999999999</v>
+        <v>0.215</v>
       </c>
       <c r="AE4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.22500000000000001</v>
+        <v>0.32</v>
       </c>
       <c r="AF4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.36499999999999999</v>
+        <v>0.27</v>
       </c>
       <c r="AG4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.22</v>
+        <v>0.315</v>
       </c>
       <c r="AH4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.28999999999999998</v>
+        <v>0.25</v>
       </c>
       <c r="AI4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.16875000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.30625000000000002</v>
+        <v>0.15</v>
       </c>
       <c r="AK4" s="1">
         <f t="shared" si="2"/>
@@ -1554,31 +1554,31 @@
       </c>
       <c r="AL4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.21875</v>
+        <v>0.26874999999999999</v>
       </c>
       <c r="AM4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.28125</v>
+        <v>0.4</v>
       </c>
       <c r="AN4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.45624999999999999</v>
+        <v>0.33750000000000002</v>
       </c>
       <c r="AO4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.27500000000000002</v>
+        <v>0.39374999999999999</v>
       </c>
       <c r="AP4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.36249999999999999</v>
+        <v>0.3125</v>
       </c>
       <c r="AQ4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.20250000000000001</v>
+        <v>0.18</v>
       </c>
       <c r="AR4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.36749999999999999</v>
+        <v>0.18</v>
       </c>
       <c r="AS4" s="1">
         <f t="shared" si="2"/>
@@ -1586,31 +1586,31 @@
       </c>
       <c r="AT4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.26249999999999996</v>
+        <v>0.32250000000000001</v>
       </c>
       <c r="AU4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.33750000000000002</v>
+        <v>0.48</v>
       </c>
       <c r="AV4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.54749999999999999</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="AW4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.33</v>
+        <v>0.47250000000000003</v>
       </c>
       <c r="AX4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.43499999999999994</v>
+        <v>0.375</v>
       </c>
       <c r="AY4" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>6.7500000000000004E-2</v>
+        <v>0.06</v>
       </c>
       <c r="AZ4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1225</v>
+        <v>0.06</v>
       </c>
       <c r="BA4" s="1">
         <f t="shared" si="3"/>
@@ -1618,31 +1618,31 @@
       </c>
       <c r="BB4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>8.7499999999999994E-2</v>
+        <v>0.1075</v>
       </c>
       <c r="BC4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1125</v>
+        <v>0.16</v>
       </c>
       <c r="BD4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1825</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="BE4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.11</v>
+        <v>0.1575</v>
       </c>
       <c r="BF4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14499999999999999</v>
+        <v>0.125</v>
       </c>
       <c r="BG4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>8.4375000000000006E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="BH4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.15312500000000001</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="BI4" s="1">
         <f t="shared" si="3"/>
@@ -1650,31 +1650,31 @@
       </c>
       <c r="BJ4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.109375</v>
+        <v>0.13437499999999999</v>
       </c>
       <c r="BK4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.140625</v>
+        <v>0.2</v>
       </c>
       <c r="BL4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22812499999999999</v>
+        <v>0.16875000000000001</v>
       </c>
       <c r="BM4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.13750000000000001</v>
+        <v>0.19687499999999999</v>
       </c>
       <c r="BN4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.18124999999999999</v>
+        <v>0.15625</v>
       </c>
       <c r="BO4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.10125000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="BP4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.18375</v>
+        <v>0.09</v>
       </c>
       <c r="BQ4" s="1">
         <f t="shared" si="3"/>
@@ -1682,23 +1682,23 @@
       </c>
       <c r="BR4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.13124999999999998</v>
+        <v>0.16125</v>
       </c>
       <c r="BS4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.16875000000000001</v>
+        <v>0.24</v>
       </c>
       <c r="BT4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.27374999999999999</v>
+        <v>0.20250000000000001</v>
       </c>
       <c r="BU4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.16500000000000001</v>
+        <v>0.23625000000000002</v>
       </c>
       <c r="BV4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.21749999999999997</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="5" spans="1:74" x14ac:dyDescent="0.25">
@@ -1710,46 +1710,46 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">F2</f>
-        <v>0.42</v>
+        <v>0.1</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">F3</f>
-        <v>0.46</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="E5" s="1">
         <f ca="1">F4</f>
-        <v>0.35</v>
+        <v>0.43</v>
       </c>
       <c r="F5" s="2">
         <v>0.4</v>
       </c>
       <c r="G5" s="1">
         <f ca="1">RANDBETWEEN(MIN($E5, G6)*100, ($E5+G6)*100)/100</f>
-        <v>0.62</v>
+        <v>0.9</v>
       </c>
       <c r="H5" s="1">
         <f ca="1">RANDBETWEEN(MIN($E5, H7)*100, ($E5+H7)*100)/100</f>
-        <v>0.53</v>
+        <v>0.97</v>
       </c>
       <c r="I5" s="1">
         <f ca="1">RANDBETWEEN(MIN($E5, I8)*100, ($E5+I8)*100)/100</f>
-        <v>0.85</v>
+        <v>0.49</v>
       </c>
       <c r="J5" s="1">
         <f ca="1">RANDBETWEEN(MIN($E5, J9)*100, ($E5+J9)*100)/100</f>
-        <v>0.71</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="K5" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.52500000000000002</v>
+        <v>0.125</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0.57500000000000007</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>0.4375</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" si="7"/>
@@ -1757,31 +1757,31 @@
       </c>
       <c r="O5" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>0.77500000000000002</v>
+        <v>1.125</v>
       </c>
       <c r="P5" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.66250000000000009</v>
+        <v>1.2124999999999999</v>
       </c>
       <c r="Q5" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>1.0625</v>
+        <v>0.61250000000000004</v>
       </c>
       <c r="R5" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0.88749999999999996</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="S5" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>0.63</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="T5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69000000000000006</v>
+        <v>0.84000000000000008</v>
       </c>
       <c r="U5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52499999999999991</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="V5" s="1">
         <f t="shared" si="1"/>
@@ -1789,31 +1789,31 @@
       </c>
       <c r="W5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92999999999999994</v>
+        <v>1.35</v>
       </c>
       <c r="X5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.79500000000000004</v>
+        <v>1.4550000000000001</v>
       </c>
       <c r="Y5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2749999999999999</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="Z5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0649999999999999</v>
+        <v>0.86999999999999988</v>
       </c>
       <c r="AA5" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>0.21</v>
+        <v>0.05</v>
       </c>
       <c r="AB5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.23</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AC5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.17499999999999999</v>
+        <v>0.215</v>
       </c>
       <c r="AD5" s="1">
         <f t="shared" si="2"/>
@@ -1821,31 +1821,31 @@
       </c>
       <c r="AE5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.31</v>
+        <v>0.45</v>
       </c>
       <c r="AF5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.26500000000000001</v>
+        <v>0.48499999999999999</v>
       </c>
       <c r="AG5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.42499999999999999</v>
+        <v>0.245</v>
       </c>
       <c r="AH5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.35499999999999998</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="AI5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.26250000000000001</v>
+        <v>6.25E-2</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.28750000000000003</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="AK5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.21875</v>
+        <v>0.26874999999999999</v>
       </c>
       <c r="AL5" s="1">
         <f t="shared" si="2"/>
@@ -1853,31 +1853,31 @@
       </c>
       <c r="AM5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.38750000000000001</v>
+        <v>0.5625</v>
       </c>
       <c r="AN5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.33125000000000004</v>
+        <v>0.60624999999999996</v>
       </c>
       <c r="AO5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.53125</v>
+        <v>0.30625000000000002</v>
       </c>
       <c r="AP5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.44374999999999998</v>
+        <v>0.36249999999999999</v>
       </c>
       <c r="AQ5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.315</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="AR5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.34500000000000003</v>
+        <v>0.42000000000000004</v>
       </c>
       <c r="AS5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.26249999999999996</v>
+        <v>0.32250000000000001</v>
       </c>
       <c r="AT5" s="1">
         <f t="shared" si="2"/>
@@ -1885,31 +1885,31 @@
       </c>
       <c r="AU5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.46499999999999997</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="AV5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.39750000000000002</v>
+        <v>0.72750000000000004</v>
       </c>
       <c r="AW5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.63749999999999996</v>
+        <v>0.36749999999999999</v>
       </c>
       <c r="AX5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.53249999999999997</v>
+        <v>0.43499999999999994</v>
       </c>
       <c r="AY5" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.105</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AZ5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.115</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="BA5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>8.7499999999999994E-2</v>
+        <v>0.1075</v>
       </c>
       <c r="BB5" s="1">
         <f t="shared" si="3"/>
@@ -1917,31 +1917,31 @@
       </c>
       <c r="BC5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.155</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="BD5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.13250000000000001</v>
+        <v>0.24249999999999999</v>
       </c>
       <c r="BE5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.21249999999999999</v>
+        <v>0.1225</v>
       </c>
       <c r="BF5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.17749999999999999</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="BG5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.13125000000000001</v>
+        <v>3.125E-2</v>
       </c>
       <c r="BH5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14375000000000002</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="BI5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.109375</v>
+        <v>0.13437499999999999</v>
       </c>
       <c r="BJ5" s="1">
         <f t="shared" si="3"/>
@@ -1949,31 +1949,31 @@
       </c>
       <c r="BK5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.19375000000000001</v>
+        <v>0.28125</v>
       </c>
       <c r="BL5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.16562500000000002</v>
+        <v>0.30312499999999998</v>
       </c>
       <c r="BM5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.265625</v>
+        <v>0.15312500000000001</v>
       </c>
       <c r="BN5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22187499999999999</v>
+        <v>0.18124999999999999</v>
       </c>
       <c r="BO5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1575</v>
+        <v>3.7500000000000006E-2</v>
       </c>
       <c r="BP5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.17250000000000001</v>
+        <v>0.21000000000000002</v>
       </c>
       <c r="BQ5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.13124999999999998</v>
+        <v>0.16125</v>
       </c>
       <c r="BR5" s="1">
         <f t="shared" si="3"/>
@@ -1981,19 +1981,19 @@
       </c>
       <c r="BS5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.23249999999999998</v>
+        <v>0.33750000000000002</v>
       </c>
       <c r="BT5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.19875000000000001</v>
+        <v>0.36375000000000002</v>
       </c>
       <c r="BU5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.31874999999999998</v>
+        <v>0.18375</v>
       </c>
       <c r="BV5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.26624999999999999</v>
+        <v>0.21749999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:74" x14ac:dyDescent="0.25">
@@ -2005,50 +2005,50 @@
       </c>
       <c r="C6" s="1">
         <f ca="1">G2</f>
-        <v>0.16</v>
+        <v>0.59</v>
       </c>
       <c r="D6" s="1">
         <f ca="1">G3</f>
-        <v>0.56000000000000005</v>
+        <v>0.51</v>
       </c>
       <c r="E6" s="1">
         <f ca="1">G4</f>
-        <v>0.45</v>
+        <v>0.64</v>
       </c>
       <c r="F6" s="1">
         <f ca="1">G5</f>
-        <v>0.62</v>
+        <v>0.9</v>
       </c>
       <c r="G6" s="2">
         <v>0.5</v>
       </c>
       <c r="H6" s="1">
         <f ca="1">RANDBETWEEN(MIN($G6, H7)*100, ($G6+H7)*100)/100</f>
-        <v>0.88</v>
+        <v>0.53</v>
       </c>
       <c r="I6" s="1">
         <f ca="1">RANDBETWEEN(MIN($G6, I8)*100, ($G6+I8)*100)/100</f>
-        <v>0.75</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="J6" s="1">
         <f ca="1">RANDBETWEEN(MIN($G6, J9)*100, ($G6+J9)*100)/100</f>
-        <v>0.72</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="K6" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.2</v>
+        <v>0.73749999999999993</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0.70000000000000007</v>
+        <v>0.63749999999999996</v>
       </c>
       <c r="M6" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>0.5625</v>
+        <v>0.8</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>0.77500000000000002</v>
+        <v>1.125</v>
       </c>
       <c r="O6" s="1">
         <f t="shared" si="8"/>
@@ -2056,31 +2056,31 @@
       </c>
       <c r="P6" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>1.1000000000000001</v>
+        <v>0.66250000000000009</v>
       </c>
       <c r="Q6" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>0.9375</v>
+        <v>1.45</v>
       </c>
       <c r="R6" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0.89999999999999991</v>
+        <v>1.3625</v>
       </c>
       <c r="S6" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>0.24</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="T6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.84000000000000008</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="U6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67500000000000004</v>
+        <v>0.96</v>
       </c>
       <c r="V6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92999999999999994</v>
+        <v>1.35</v>
       </c>
       <c r="W6" s="1">
         <f t="shared" si="1"/>
@@ -2088,31 +2088,31 @@
       </c>
       <c r="X6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.32</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="Y6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.125</v>
+        <v>1.7399999999999998</v>
       </c>
       <c r="Z6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.08</v>
+        <v>1.6350000000000002</v>
       </c>
       <c r="AA6" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>0.08</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="AB6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.28000000000000003</v>
+        <v>0.255</v>
       </c>
       <c r="AC6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.22500000000000001</v>
+        <v>0.32</v>
       </c>
       <c r="AD6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.31</v>
+        <v>0.45</v>
       </c>
       <c r="AE6" s="1">
         <f t="shared" si="2"/>
@@ -2120,31 +2120,31 @@
       </c>
       <c r="AF6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.44</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="AG6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.375</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="AH6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.36</v>
+        <v>0.54500000000000004</v>
       </c>
       <c r="AI6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.1</v>
+        <v>0.36874999999999997</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.35000000000000003</v>
+        <v>0.31874999999999998</v>
       </c>
       <c r="AK6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.28125</v>
+        <v>0.4</v>
       </c>
       <c r="AL6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.38750000000000001</v>
+        <v>0.5625</v>
       </c>
       <c r="AM6" s="1">
         <f t="shared" si="2"/>
@@ -2152,31 +2152,31 @@
       </c>
       <c r="AN6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.33125000000000004</v>
       </c>
       <c r="AO6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.46875</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="AP6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.44999999999999996</v>
+        <v>0.68125000000000002</v>
       </c>
       <c r="AQ6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.12</v>
+        <v>0.4425</v>
       </c>
       <c r="AR6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.42000000000000004</v>
+        <v>0.38250000000000001</v>
       </c>
       <c r="AS6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.33750000000000002</v>
+        <v>0.48</v>
       </c>
       <c r="AT6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.46499999999999997</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="AU6" s="1">
         <f t="shared" si="2"/>
@@ -2184,31 +2184,31 @@
       </c>
       <c r="AV6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.66</v>
+        <v>0.39750000000000002</v>
       </c>
       <c r="AW6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.5625</v>
+        <v>0.86999999999999988</v>
       </c>
       <c r="AX6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.54</v>
+        <v>0.81750000000000012</v>
       </c>
       <c r="AY6" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.04</v>
+        <v>0.14749999999999999</v>
       </c>
       <c r="AZ6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14000000000000001</v>
+        <v>0.1275</v>
       </c>
       <c r="BA6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1125</v>
+        <v>0.16</v>
       </c>
       <c r="BB6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.155</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="BC6" s="1">
         <f t="shared" si="3"/>
@@ -2216,31 +2216,31 @@
       </c>
       <c r="BD6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22</v>
+        <v>0.13250000000000001</v>
       </c>
       <c r="BE6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1875</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="BF6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.18</v>
+        <v>0.27250000000000002</v>
       </c>
       <c r="BG6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.05</v>
+        <v>0.18437499999999998</v>
       </c>
       <c r="BH6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.17500000000000002</v>
+        <v>0.15937499999999999</v>
       </c>
       <c r="BI6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.140625</v>
+        <v>0.2</v>
       </c>
       <c r="BJ6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.19375000000000001</v>
+        <v>0.28125</v>
       </c>
       <c r="BK6" s="1">
         <f t="shared" si="3"/>
@@ -2248,31 +2248,31 @@
       </c>
       <c r="BL6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.27500000000000002</v>
+        <v>0.16562500000000002</v>
       </c>
       <c r="BM6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.234375</v>
+        <v>0.36249999999999999</v>
       </c>
       <c r="BN6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22499999999999998</v>
+        <v>0.34062500000000001</v>
       </c>
       <c r="BO6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.06</v>
+        <v>0.22125</v>
       </c>
       <c r="BP6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.21000000000000002</v>
+        <v>0.19125</v>
       </c>
       <c r="BQ6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.16875000000000001</v>
+        <v>0.24</v>
       </c>
       <c r="BR6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.23249999999999998</v>
+        <v>0.33750000000000002</v>
       </c>
       <c r="BS6" s="1">
         <f t="shared" si="3"/>
@@ -2280,15 +2280,15 @@
       </c>
       <c r="BT6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.33</v>
+        <v>0.19875000000000001</v>
       </c>
       <c r="BU6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.28125</v>
+        <v>0.43499999999999994</v>
       </c>
       <c r="BV6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.27</v>
+        <v>0.40875000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:74" x14ac:dyDescent="0.25">
@@ -2300,54 +2300,54 @@
       </c>
       <c r="C7" s="1">
         <f ca="1">H2</f>
-        <v>0.28999999999999998</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D7" s="1">
         <f ca="1">H3</f>
-        <v>0.41</v>
+        <v>0.78</v>
       </c>
       <c r="E7" s="1">
         <f ca="1">H4</f>
-        <v>0.73</v>
+        <v>0.54</v>
       </c>
       <c r="F7" s="1">
         <f ca="1">H5</f>
-        <v>0.53</v>
+        <v>0.97</v>
       </c>
       <c r="G7" s="1">
         <f ca="1">H6</f>
-        <v>0.88</v>
+        <v>0.53</v>
       </c>
       <c r="H7" s="2">
         <v>0.6</v>
       </c>
       <c r="I7" s="1">
         <f ca="1">RANDBETWEEN(MIN($G7, I8)*100, ($G7+I8)*100)/100</f>
-        <v>0.73</v>
+        <v>0.67</v>
       </c>
       <c r="J7" s="1">
         <f ca="1">RANDBETWEEN(MIN($G7, J9)*100, ($G7+J9)*100)/100</f>
-        <v>1.1299999999999999</v>
+        <v>0.79</v>
       </c>
       <c r="K7" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.36249999999999999</v>
+        <v>0.6875</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0.51249999999999996</v>
+        <v>0.97500000000000009</v>
       </c>
       <c r="M7" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>0.91249999999999998</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>0.66250000000000009</v>
+        <v>1.2124999999999999</v>
       </c>
       <c r="O7" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>1.1000000000000001</v>
+        <v>0.66250000000000009</v>
       </c>
       <c r="P7" s="1">
         <f t="shared" si="9"/>
@@ -2355,31 +2355,31 @@
       </c>
       <c r="Q7" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>0.91249999999999998</v>
+        <v>0.83750000000000002</v>
       </c>
       <c r="R7" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>1.4124999999999999</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="S7" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>0.43499999999999994</v>
+        <v>0.82500000000000007</v>
       </c>
       <c r="T7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61499999999999999</v>
+        <v>1.17</v>
       </c>
       <c r="U7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.095</v>
+        <v>0.81</v>
       </c>
       <c r="V7" s="1">
         <f t="shared" ca="1" si="1"/>
+        <v>1.4550000000000001</v>
+      </c>
+      <c r="W7" s="1">
+        <f t="shared" ca="1" si="1"/>
         <v>0.79500000000000004</v>
-      </c>
-      <c r="W7" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.32</v>
       </c>
       <c r="X7" s="1">
         <f t="shared" si="1"/>
@@ -2387,31 +2387,31 @@
       </c>
       <c r="Y7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.095</v>
+        <v>1.0050000000000001</v>
       </c>
       <c r="Z7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6949999999999998</v>
+        <v>1.1850000000000001</v>
       </c>
       <c r="AA7" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>0.14499999999999999</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="AB7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.20499999999999999</v>
+        <v>0.39</v>
       </c>
       <c r="AC7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.36499999999999999</v>
+        <v>0.27</v>
       </c>
       <c r="AD7" s="1">
         <f t="shared" ca="1" si="2"/>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="AE7" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>0.26500000000000001</v>
-      </c>
-      <c r="AE7" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.44</v>
       </c>
       <c r="AF7" s="1">
         <f t="shared" si="2"/>
@@ -2419,31 +2419,31 @@
       </c>
       <c r="AG7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.36499999999999999</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="AH7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.56499999999999995</v>
+        <v>0.39500000000000002</v>
       </c>
       <c r="AI7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.18124999999999999</v>
+        <v>0.34375</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.25624999999999998</v>
+        <v>0.48750000000000004</v>
       </c>
       <c r="AK7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.45624999999999999</v>
+        <v>0.33750000000000002</v>
       </c>
       <c r="AL7" s="1">
         <f t="shared" ca="1" si="2"/>
+        <v>0.60624999999999996</v>
+      </c>
+      <c r="AM7" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>0.33125000000000004</v>
-      </c>
-      <c r="AM7" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.55000000000000004</v>
       </c>
       <c r="AN7" s="1">
         <f t="shared" si="2"/>
@@ -2451,31 +2451,31 @@
       </c>
       <c r="AO7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.45624999999999999</v>
+        <v>0.41875000000000001</v>
       </c>
       <c r="AP7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.70624999999999993</v>
+        <v>0.49375000000000002</v>
       </c>
       <c r="AQ7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.21749999999999997</v>
+        <v>0.41250000000000003</v>
       </c>
       <c r="AR7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.3075</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="AS7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.54749999999999999</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="AT7" s="1">
         <f t="shared" ca="1" si="2"/>
+        <v>0.72750000000000004</v>
+      </c>
+      <c r="AU7" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>0.39750000000000002</v>
-      </c>
-      <c r="AU7" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.66</v>
       </c>
       <c r="AV7" s="1">
         <f t="shared" si="2"/>
@@ -2483,31 +2483,31 @@
       </c>
       <c r="AW7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.54749999999999999</v>
+        <v>0.50250000000000006</v>
       </c>
       <c r="AX7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.84749999999999992</v>
+        <v>0.59250000000000003</v>
       </c>
       <c r="AY7" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>7.2499999999999995E-2</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="AZ7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.10249999999999999</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="BA7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1825</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="BB7" s="1">
         <f t="shared" ca="1" si="3"/>
+        <v>0.24249999999999999</v>
+      </c>
+      <c r="BC7" s="1">
+        <f t="shared" ca="1" si="3"/>
         <v>0.13250000000000001</v>
-      </c>
-      <c r="BC7" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.22</v>
       </c>
       <c r="BD7" s="1">
         <f t="shared" si="3"/>
@@ -2515,31 +2515,31 @@
       </c>
       <c r="BE7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1825</v>
+        <v>0.16750000000000001</v>
       </c>
       <c r="BF7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.28249999999999997</v>
+        <v>0.19750000000000001</v>
       </c>
       <c r="BG7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>9.0624999999999997E-2</v>
+        <v>0.171875</v>
       </c>
       <c r="BH7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.12812499999999999</v>
+        <v>0.24375000000000002</v>
       </c>
       <c r="BI7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22812499999999999</v>
+        <v>0.16875000000000001</v>
       </c>
       <c r="BJ7" s="1">
         <f t="shared" ca="1" si="3"/>
+        <v>0.30312499999999998</v>
+      </c>
+      <c r="BK7" s="1">
+        <f t="shared" ca="1" si="3"/>
         <v>0.16562500000000002</v>
-      </c>
-      <c r="BK7" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.27500000000000002</v>
       </c>
       <c r="BL7" s="1">
         <f t="shared" si="3"/>
@@ -2547,31 +2547,31 @@
       </c>
       <c r="BM7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22812499999999999</v>
+        <v>0.20937500000000001</v>
       </c>
       <c r="BN7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.35312499999999997</v>
+        <v>0.24687500000000001</v>
       </c>
       <c r="BO7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.10874999999999999</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="BP7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.15375</v>
+        <v>0.29249999999999998</v>
       </c>
       <c r="BQ7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.27374999999999999</v>
+        <v>0.20250000000000001</v>
       </c>
       <c r="BR7" s="1">
         <f t="shared" ca="1" si="3"/>
+        <v>0.36375000000000002</v>
+      </c>
+      <c r="BS7" s="1">
+        <f t="shared" ca="1" si="3"/>
         <v>0.19875000000000001</v>
-      </c>
-      <c r="BS7" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.33</v>
       </c>
       <c r="BT7" s="1">
         <f t="shared" si="3"/>
@@ -2579,11 +2579,11 @@
       </c>
       <c r="BU7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.27374999999999999</v>
+        <v>0.25125000000000003</v>
       </c>
       <c r="BV7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.42374999999999996</v>
+        <v>0.29625000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:74" x14ac:dyDescent="0.25">
@@ -2595,58 +2595,58 @@
       </c>
       <c r="C8" s="1">
         <f ca="1">I2</f>
-        <v>0.67</v>
+        <v>0.25</v>
       </c>
       <c r="D8" s="1">
         <f ca="1">I3</f>
-        <v>0.63</v>
+        <v>0.59</v>
       </c>
       <c r="E8" s="1">
         <f ca="1">I4</f>
-        <v>0.44</v>
+        <v>0.63</v>
       </c>
       <c r="F8" s="1">
         <f ca="1">I5</f>
-        <v>0.85</v>
+        <v>0.49</v>
       </c>
       <c r="G8" s="1">
         <f ca="1">I6</f>
-        <v>0.75</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="H8" s="1">
         <f ca="1">I7</f>
-        <v>0.73</v>
+        <v>0.67</v>
       </c>
       <c r="I8" s="2">
         <v>0.7</v>
       </c>
       <c r="J8" s="1">
         <f ca="1">RANDBETWEEN(MIN(I8, J9)*100, (I8+J9)*100)/100</f>
-        <v>1.47</v>
+        <v>1.48</v>
       </c>
       <c r="K8" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.83750000000000002</v>
+        <v>0.3125</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0.78749999999999998</v>
+        <v>0.73749999999999993</v>
       </c>
       <c r="M8" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>0.55000000000000004</v>
+        <v>0.78749999999999998</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>1.0625</v>
+        <v>0.61250000000000004</v>
       </c>
       <c r="O8" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>0.9375</v>
+        <v>1.45</v>
       </c>
       <c r="P8" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0.91249999999999998</v>
+        <v>0.83750000000000002</v>
       </c>
       <c r="Q8" s="1">
         <f t="shared" si="10"/>
@@ -2654,31 +2654,31 @@
       </c>
       <c r="R8" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>1.8374999999999999</v>
+        <v>1.85</v>
       </c>
       <c r="S8" s="1">
         <f t="shared" ca="1" si="12"/>
+        <v>0.375</v>
+      </c>
+      <c r="T8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="U8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.94500000000000006</v>
+      </c>
+      <c r="V8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="W8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.7399999999999998</v>
+      </c>
+      <c r="X8" s="1">
+        <f t="shared" ca="1" si="1"/>
         <v>1.0050000000000001</v>
-      </c>
-      <c r="T8" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.94500000000000006</v>
-      </c>
-      <c r="U8" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.66</v>
-      </c>
-      <c r="V8" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.2749999999999999</v>
-      </c>
-      <c r="W8" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.125</v>
-      </c>
-      <c r="X8" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.095</v>
       </c>
       <c r="Y8" s="1">
         <f t="shared" si="1"/>
@@ -2686,31 +2686,31 @@
       </c>
       <c r="Z8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2050000000000001</v>
+        <v>2.2199999999999998</v>
       </c>
       <c r="AA8" s="1">
         <f t="shared" ca="1" si="13"/>
+        <v>0.125</v>
+      </c>
+      <c r="AB8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="AC8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.315</v>
+      </c>
+      <c r="AD8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.245</v>
+      </c>
+      <c r="AE8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AF8" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>0.33500000000000002</v>
-      </c>
-      <c r="AB8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.315</v>
-      </c>
-      <c r="AC8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.22</v>
-      </c>
-      <c r="AD8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="AE8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.375</v>
-      </c>
-      <c r="AF8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.36499999999999999</v>
       </c>
       <c r="AG8" s="1">
         <f t="shared" si="2"/>
@@ -2718,31 +2718,31 @@
       </c>
       <c r="AH8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.73499999999999999</v>
+        <v>0.74</v>
       </c>
       <c r="AI8" s="1">
         <f t="shared" ca="1" si="2"/>
+        <v>0.15625</v>
+      </c>
+      <c r="AJ8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.36874999999999997</v>
+      </c>
+      <c r="AK8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.39374999999999999</v>
+      </c>
+      <c r="AL8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.30625000000000002</v>
+      </c>
+      <c r="AM8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="AN8" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>0.41875000000000001</v>
-      </c>
-      <c r="AJ8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.39374999999999999</v>
-      </c>
-      <c r="AK8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="AL8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.53125</v>
-      </c>
-      <c r="AM8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.46875</v>
-      </c>
-      <c r="AN8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.45624999999999999</v>
       </c>
       <c r="AO8" s="1">
         <f t="shared" si="2"/>
@@ -2750,31 +2750,31 @@
       </c>
       <c r="AP8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.91874999999999996</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="AQ8" s="1">
         <f t="shared" ca="1" si="2"/>
+        <v>0.1875</v>
+      </c>
+      <c r="AR8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.4425</v>
+      </c>
+      <c r="AS8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.47250000000000003</v>
+      </c>
+      <c r="AT8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.36749999999999999</v>
+      </c>
+      <c r="AU8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.86999999999999988</v>
+      </c>
+      <c r="AV8" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>0.50250000000000006</v>
-      </c>
-      <c r="AR8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.47250000000000003</v>
-      </c>
-      <c r="AS8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.33</v>
-      </c>
-      <c r="AT8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.63749999999999996</v>
-      </c>
-      <c r="AU8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.5625</v>
-      </c>
-      <c r="AV8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.54749999999999999</v>
       </c>
       <c r="AW8" s="1">
         <f t="shared" si="2"/>
@@ -2782,31 +2782,31 @@
       </c>
       <c r="AX8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1.1025</v>
+        <v>1.1099999999999999</v>
       </c>
       <c r="AY8" s="1">
         <f t="shared" ca="1" si="14"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="AZ8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.14749999999999999</v>
+      </c>
+      <c r="BA8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.1575</v>
+      </c>
+      <c r="BB8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.1225</v>
+      </c>
+      <c r="BC8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="BD8" s="1">
+        <f t="shared" ca="1" si="3"/>
         <v>0.16750000000000001</v>
-      </c>
-      <c r="AZ8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.1575</v>
-      </c>
-      <c r="BA8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.11</v>
-      </c>
-      <c r="BB8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.21249999999999999</v>
-      </c>
-      <c r="BC8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.1875</v>
-      </c>
-      <c r="BD8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.1825</v>
       </c>
       <c r="BE8" s="1">
         <f t="shared" si="3"/>
@@ -2814,31 +2814,31 @@
       </c>
       <c r="BF8" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.36749999999999999</v>
+        <v>0.37</v>
       </c>
       <c r="BG8" s="1">
         <f t="shared" ca="1" si="3"/>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="BH8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.18437499999999998</v>
+      </c>
+      <c r="BI8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.19687499999999999</v>
+      </c>
+      <c r="BJ8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.15312500000000001</v>
+      </c>
+      <c r="BK8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="BL8" s="1">
+        <f t="shared" ca="1" si="3"/>
         <v>0.20937500000000001</v>
-      </c>
-      <c r="BH8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.19687499999999999</v>
-      </c>
-      <c r="BI8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.13750000000000001</v>
-      </c>
-      <c r="BJ8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.265625</v>
-      </c>
-      <c r="BK8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.234375</v>
-      </c>
-      <c r="BL8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.22812499999999999</v>
       </c>
       <c r="BM8" s="1">
         <f t="shared" si="3"/>
@@ -2846,31 +2846,31 @@
       </c>
       <c r="BN8" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.45937499999999998</v>
+        <v>0.46250000000000002</v>
       </c>
       <c r="BO8" s="1">
         <f t="shared" ca="1" si="3"/>
+        <v>9.375E-2</v>
+      </c>
+      <c r="BP8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.22125</v>
+      </c>
+      <c r="BQ8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.23625000000000002</v>
+      </c>
+      <c r="BR8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.18375</v>
+      </c>
+      <c r="BS8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.43499999999999994</v>
+      </c>
+      <c r="BT8" s="1">
+        <f t="shared" ca="1" si="3"/>
         <v>0.25125000000000003</v>
-      </c>
-      <c r="BP8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.23625000000000002</v>
-      </c>
-      <c r="BQ8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="BR8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.31874999999999998</v>
-      </c>
-      <c r="BS8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.28125</v>
-      </c>
-      <c r="BT8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.27374999999999999</v>
       </c>
       <c r="BU8" s="1">
         <f t="shared" si="3"/>
@@ -2878,7 +2878,7 @@
       </c>
       <c r="BV8" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.55125000000000002</v>
+        <v>0.55499999999999994</v>
       </c>
     </row>
     <row r="9" spans="1:74" x14ac:dyDescent="0.25">
@@ -2890,62 +2890,62 @@
       </c>
       <c r="C9" s="1">
         <f ca="1">J2</f>
-        <v>0.17</v>
+        <v>0.61</v>
       </c>
       <c r="D9" s="1">
         <f ca="1">J3</f>
-        <v>0.47</v>
+        <v>0.37</v>
       </c>
       <c r="E9" s="1">
         <f ca="1">J4</f>
-        <v>0.57999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="F9" s="1">
         <f ca="1">J5</f>
-        <v>0.71</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G9" s="1">
         <f ca="1">J6</f>
-        <v>0.72</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="H9" s="1">
         <f ca="1">J7</f>
-        <v>1.1299999999999999</v>
+        <v>0.79</v>
       </c>
       <c r="I9" s="1">
         <f ca="1">J8</f>
-        <v>1.47</v>
+        <v>1.48</v>
       </c>
       <c r="J9" s="2">
         <v>0.8</v>
       </c>
       <c r="K9" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.21250000000000002</v>
+        <v>0.76249999999999996</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0.58749999999999991</v>
+        <v>0.46250000000000002</v>
       </c>
       <c r="M9" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>0.72499999999999998</v>
+        <v>0.625</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>0.88749999999999996</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="O9" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>0.89999999999999991</v>
+        <v>1.3625</v>
       </c>
       <c r="P9" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>1.4124999999999999</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="Q9" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>1.8374999999999999</v>
+        <v>1.85</v>
       </c>
       <c r="R9" s="1">
         <f t="shared" si="11"/>
@@ -2953,31 +2953,31 @@
       </c>
       <c r="S9" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>0.255</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="T9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70499999999999996</v>
+        <v>0.55499999999999994</v>
       </c>
       <c r="U9" s="1">
         <f t="shared" ca="1" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="V9" s="1">
+        <f t="shared" ca="1" si="1"/>
         <v>0.86999999999999988</v>
       </c>
-      <c r="V9" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.0649999999999999</v>
-      </c>
       <c r="W9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.08</v>
+        <v>1.6350000000000002</v>
       </c>
       <c r="X9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6949999999999998</v>
+        <v>1.1850000000000001</v>
       </c>
       <c r="Y9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2050000000000001</v>
+        <v>2.2199999999999998</v>
       </c>
       <c r="Z9" s="1">
         <f t="shared" si="1"/>
@@ -2985,31 +2985,31 @@
       </c>
       <c r="AA9" s="1">
         <f t="shared" ca="1" si="13"/>
-        <v>8.5000000000000006E-2</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="AB9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.23499999999999999</v>
+        <v>0.185</v>
       </c>
       <c r="AC9" s="1">
         <f t="shared" ca="1" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="AD9" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>0.28999999999999998</v>
       </c>
-      <c r="AD9" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.35499999999999998</v>
-      </c>
       <c r="AE9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.36</v>
+        <v>0.54500000000000004</v>
       </c>
       <c r="AF9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.56499999999999995</v>
+        <v>0.39500000000000002</v>
       </c>
       <c r="AG9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.73499999999999999</v>
+        <v>0.74</v>
       </c>
       <c r="AH9" s="1">
         <f t="shared" si="2"/>
@@ -3017,31 +3017,31 @@
       </c>
       <c r="AI9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.10625000000000001</v>
+        <v>0.38124999999999998</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.29374999999999996</v>
+        <v>0.23125000000000001</v>
       </c>
       <c r="AK9" s="1">
         <f t="shared" ca="1" si="2"/>
+        <v>0.3125</v>
+      </c>
+      <c r="AL9" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>0.36249999999999999</v>
       </c>
-      <c r="AL9" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.44374999999999998</v>
-      </c>
       <c r="AM9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.44999999999999996</v>
+        <v>0.68125000000000002</v>
       </c>
       <c r="AN9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.70624999999999993</v>
+        <v>0.49375000000000002</v>
       </c>
       <c r="AO9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.91874999999999996</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="AP9" s="1">
         <f t="shared" si="2"/>
@@ -3049,31 +3049,31 @@
       </c>
       <c r="AQ9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.1275</v>
+        <v>0.45750000000000002</v>
       </c>
       <c r="AR9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.35249999999999998</v>
+        <v>0.27749999999999997</v>
       </c>
       <c r="AS9" s="1">
         <f t="shared" ca="1" si="2"/>
+        <v>0.375</v>
+      </c>
+      <c r="AT9" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>0.43499999999999994</v>
       </c>
-      <c r="AT9" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.53249999999999997</v>
-      </c>
       <c r="AU9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.54</v>
+        <v>0.81750000000000012</v>
       </c>
       <c r="AV9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.84749999999999992</v>
+        <v>0.59250000000000003</v>
       </c>
       <c r="AW9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1.1025</v>
+        <v>1.1099999999999999</v>
       </c>
       <c r="AX9" s="1">
         <f t="shared" si="2"/>
@@ -3081,31 +3081,31 @@
       </c>
       <c r="AY9" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>4.2500000000000003E-2</v>
+        <v>0.1525</v>
       </c>
       <c r="AZ9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.11749999999999999</v>
+        <v>9.2499999999999999E-2</v>
       </c>
       <c r="BA9" s="1">
         <f t="shared" ca="1" si="3"/>
+        <v>0.125</v>
+      </c>
+      <c r="BB9" s="1">
+        <f t="shared" ca="1" si="3"/>
         <v>0.14499999999999999</v>
       </c>
-      <c r="BB9" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.17749999999999999</v>
-      </c>
       <c r="BC9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.18</v>
+        <v>0.27250000000000002</v>
       </c>
       <c r="BD9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.28249999999999997</v>
+        <v>0.19750000000000001</v>
       </c>
       <c r="BE9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.36749999999999999</v>
+        <v>0.37</v>
       </c>
       <c r="BF9" s="1">
         <f t="shared" si="3"/>
@@ -3113,31 +3113,31 @@
       </c>
       <c r="BG9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>5.3125000000000006E-2</v>
+        <v>0.19062499999999999</v>
       </c>
       <c r="BH9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14687499999999998</v>
+        <v>0.11562500000000001</v>
       </c>
       <c r="BI9" s="1">
         <f t="shared" ca="1" si="3"/>
+        <v>0.15625</v>
+      </c>
+      <c r="BJ9" s="1">
+        <f t="shared" ca="1" si="3"/>
         <v>0.18124999999999999</v>
       </c>
-      <c r="BJ9" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.22187499999999999</v>
-      </c>
       <c r="BK9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22499999999999998</v>
+        <v>0.34062500000000001</v>
       </c>
       <c r="BL9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.35312499999999997</v>
+        <v>0.24687500000000001</v>
       </c>
       <c r="BM9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.45937499999999998</v>
+        <v>0.46250000000000002</v>
       </c>
       <c r="BN9" s="1">
         <f t="shared" si="3"/>
@@ -3145,31 +3145,31 @@
       </c>
       <c r="BO9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>6.3750000000000001E-2</v>
+        <v>0.22875000000000001</v>
       </c>
       <c r="BP9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.17624999999999999</v>
+        <v>0.13874999999999998</v>
       </c>
       <c r="BQ9" s="1">
         <f t="shared" ca="1" si="3"/>
+        <v>0.1875</v>
+      </c>
+      <c r="BR9" s="1">
+        <f t="shared" ca="1" si="3"/>
         <v>0.21749999999999997</v>
       </c>
-      <c r="BR9" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.26624999999999999</v>
-      </c>
       <c r="BS9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.27</v>
+        <v>0.40875000000000006</v>
       </c>
       <c r="BT9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.42374999999999996</v>
+        <v>0.29625000000000001</v>
       </c>
       <c r="BU9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.55125000000000002</v>
+        <v>0.55499999999999994</v>
       </c>
       <c r="BV9" s="1">
         <f t="shared" si="3"/>

</xml_diff>